<commit_message>
added e2e UI test scenarios, methods to actions classes,and modified TSI and BaseTest
</commit_message>
<xml_diff>
--- a/resources/templates/PageObjects/TemperatureAutomationModule.xlsx
+++ b/resources/templates/PageObjects/TemperatureAutomationModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhi1\MyHomeStudy(Automation Complete)\WorkspaceCodingAssignment\CodingAssignmentProject\CodingAssignmentProject\resources\templates\PageObjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF417AB5-AABB-4DC6-8CA0-FE24FB17219A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43E362C-C744-476E-AFBF-28AA9B20DCC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>LocatorName</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>locationTempDetailsPopup</t>
+  </si>
+  <si>
+    <t>randomLocationForScrollUse</t>
+  </si>
+  <si>
+    <t>(//div[contains(@class, 'leaflet-zoom-animated leaflet')]/div)[4]</t>
+  </si>
+  <si>
+    <t>//div[@class='leaflet-popup-content']//b[contains(text(), 'Degrees')]</t>
+  </si>
+  <si>
+    <t>degreesTemperatureOnPopup</t>
   </si>
 </sst>
 </file>
@@ -143,10 +155,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,16 +440,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" customWidth="1"/>
-    <col min="3" max="3" width="38.26953125" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="3" max="3" width="58.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -485,41 +498,58 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added API Methods(Utils) and designed main API Test
</commit_message>
<xml_diff>
--- a/resources/templates/PageObjects/TemperatureAutomationModule.xlsx
+++ b/resources/templates/PageObjects/TemperatureAutomationModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhi1\MyHomeStudy(Automation Complete)\WorkspaceCodingAssignment\CodingAssignmentProject\CodingAssignmentProject\resources\templates\PageObjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43E362C-C744-476E-AFBF-28AA9B20DCC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A687B09-E0BF-4EF0-8BFD-FA2453AF0697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,13 +84,13 @@
     <t>randomLocationForScrollUse</t>
   </si>
   <si>
-    <t>(//div[contains(@class, 'leaflet-zoom-animated leaflet')]/div)[4]</t>
-  </si>
-  <si>
     <t>//div[@class='leaflet-popup-content']//b[contains(text(), 'Degrees')]</t>
   </si>
   <si>
     <t>degreesTemperatureOnPopup</t>
+  </si>
+  <si>
+    <t>//a[@title='Zoom out']</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,7 +504,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -542,13 +542,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>